<commit_message>
Data downloaded from 11 airports :)
</commit_message>
<xml_diff>
--- a/DataBase/BZG_Arrivals.xlsx
+++ b/DataBase/BZG_Arrivals.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="63">
   <si>
     <t>NUMBER</t>
   </si>
@@ -186,6 +186,21 @@
   </si>
   <si>
     <t>0 hours, -3 minutes</t>
+  </si>
+  <si>
+    <t>9:20 PM</t>
+  </si>
+  <si>
+    <t>FR6623</t>
+  </si>
+  <si>
+    <t>(EI-EBZ)</t>
+  </si>
+  <si>
+    <t>9:07 PM</t>
+  </si>
+  <si>
+    <t>0 hours, -13 minutes</t>
   </si>
 </sst>
 </file>
@@ -230,7 +245,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:M7"/>
+  <dimension ref="A1:M8"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -493,6 +508,43 @@
       </c>
       <c r="M7" s="0"/>
     </row>
+    <row r="8">
+      <c r="A8" t="n" s="0">
+        <v>7.0</v>
+      </c>
+      <c r="B8" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="C8" t="s" s="0">
+        <v>58</v>
+      </c>
+      <c r="D8" t="s" s="0">
+        <v>59</v>
+      </c>
+      <c r="E8" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="F8" t="s" s="0">
+        <v>36</v>
+      </c>
+      <c r="G8" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="H8" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="I8" t="s" s="0">
+        <v>60</v>
+      </c>
+      <c r="J8" t="s" s="0">
+        <v>61</v>
+      </c>
+      <c r="K8" s="0"/>
+      <c r="L8" t="s" s="0">
+        <v>62</v>
+      </c>
+      <c r="M8" s="0"/>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
scraping better with date
</commit_message>
<xml_diff>
--- a/DataBase/BZG_Arrivals.xlsx
+++ b/DataBase/BZG_Arrivals.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="75">
   <si>
     <t>NUMBER</t>
   </si>
@@ -225,6 +225,18 @@
   </si>
   <si>
     <t>0 hours, -30 minutes</t>
+  </si>
+  <si>
+    <t>E170</t>
+  </si>
+  <si>
+    <t>(SP-LDF)</t>
+  </si>
+  <si>
+    <t>2:41 PM</t>
+  </si>
+  <si>
+    <t>0 hours, 11 minutes</t>
   </si>
 </sst>
 </file>
@@ -269,7 +281,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:M9"/>
+  <dimension ref="A1:M10"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -606,6 +618,43 @@
       </c>
       <c r="M9" s="0"/>
     </row>
+    <row r="10">
+      <c r="A10" t="n" s="0">
+        <v>9.0</v>
+      </c>
+      <c r="B10" t="s" s="0">
+        <v>63</v>
+      </c>
+      <c r="C10" t="s" s="0">
+        <v>51</v>
+      </c>
+      <c r="D10" t="s" s="0">
+        <v>52</v>
+      </c>
+      <c r="E10" t="s" s="0">
+        <v>44</v>
+      </c>
+      <c r="F10" t="s" s="0">
+        <v>45</v>
+      </c>
+      <c r="G10" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="H10" t="s" s="0">
+        <v>71</v>
+      </c>
+      <c r="I10" t="s" s="0">
+        <v>72</v>
+      </c>
+      <c r="J10" t="s" s="0">
+        <v>73</v>
+      </c>
+      <c r="K10" s="0"/>
+      <c r="L10" t="s" s="0">
+        <v>74</v>
+      </c>
+      <c r="M10" s="0"/>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
data + gui welcome page done
</commit_message>
<xml_diff>
--- a/DataBase/BZG_Arrivals.xlsx
+++ b/DataBase/BZG_Arrivals.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="88">
   <si>
     <t>NUMBER</t>
   </si>
@@ -237,6 +237,45 @@
   </si>
   <si>
     <t>0 hours, 11 minutes</t>
+  </si>
+  <si>
+    <t>Tuesday, Jan 10</t>
+  </si>
+  <si>
+    <t>9:00 AM</t>
+  </si>
+  <si>
+    <t>(EI-DLH)</t>
+  </si>
+  <si>
+    <t>8:36 AM</t>
+  </si>
+  <si>
+    <t>0 hours, -24 minutes</t>
+  </si>
+  <si>
+    <t>2:40 PM</t>
+  </si>
+  <si>
+    <t>2:26 PM</t>
+  </si>
+  <si>
+    <t>0 hours, -14 minutes</t>
+  </si>
+  <si>
+    <t>7:30 PM</t>
+  </si>
+  <si>
+    <t>A321</t>
+  </si>
+  <si>
+    <t>(G-WUKI)</t>
+  </si>
+  <si>
+    <t>7:09 PM</t>
+  </si>
+  <si>
+    <t>0 hours, -21 minutes</t>
   </si>
 </sst>
 </file>
@@ -281,7 +320,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:M10"/>
+  <dimension ref="A1:M13"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -655,6 +694,117 @@
       </c>
       <c r="M10" s="0"/>
     </row>
+    <row r="11">
+      <c r="A11" t="n" s="0">
+        <v>10.0</v>
+      </c>
+      <c r="B11" t="s" s="0">
+        <v>75</v>
+      </c>
+      <c r="C11" t="s" s="0">
+        <v>76</v>
+      </c>
+      <c r="D11" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="E11" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="F11" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="G11" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="H11" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="I11" t="s" s="0">
+        <v>77</v>
+      </c>
+      <c r="J11" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="K11" s="0"/>
+      <c r="L11" t="s" s="0">
+        <v>79</v>
+      </c>
+      <c r="M11" s="0"/>
+    </row>
+    <row r="12">
+      <c r="A12" t="n" s="0">
+        <v>11.0</v>
+      </c>
+      <c r="B12" t="s" s="0">
+        <v>75</v>
+      </c>
+      <c r="C12" t="s" s="0">
+        <v>80</v>
+      </c>
+      <c r="D12" t="s" s="0">
+        <v>52</v>
+      </c>
+      <c r="E12" t="s" s="0">
+        <v>44</v>
+      </c>
+      <c r="F12" t="s" s="0">
+        <v>45</v>
+      </c>
+      <c r="G12" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="H12" t="s" s="0">
+        <v>71</v>
+      </c>
+      <c r="I12" t="s" s="0">
+        <v>72</v>
+      </c>
+      <c r="J12" t="s" s="0">
+        <v>81</v>
+      </c>
+      <c r="K12" s="0"/>
+      <c r="L12" t="s" s="0">
+        <v>82</v>
+      </c>
+      <c r="M12" s="0"/>
+    </row>
+    <row r="13">
+      <c r="A13" t="n" s="0">
+        <v>12.0</v>
+      </c>
+      <c r="B13" t="s" s="0">
+        <v>75</v>
+      </c>
+      <c r="C13" t="s" s="0">
+        <v>83</v>
+      </c>
+      <c r="D13" t="s" s="0">
+        <v>35</v>
+      </c>
+      <c r="E13" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="F13" t="s" s="0">
+        <v>36</v>
+      </c>
+      <c r="G13" t="s" s="0">
+        <v>37</v>
+      </c>
+      <c r="H13" t="s" s="0">
+        <v>84</v>
+      </c>
+      <c r="I13" t="s" s="0">
+        <v>85</v>
+      </c>
+      <c r="J13" t="s" s="0">
+        <v>86</v>
+      </c>
+      <c r="K13" s="0"/>
+      <c r="L13" t="s" s="0">
+        <v>87</v>
+      </c>
+      <c r="M13" s="0"/>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
WORKING SWITCHNG BETWEEN WINDOWS
</commit_message>
<xml_diff>
--- a/DataBase/BZG_Arrivals.xlsx
+++ b/DataBase/BZG_Arrivals.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="113">
   <si>
     <t>NUMBER</t>
   </si>
@@ -339,6 +339,18 @@
   </si>
   <si>
     <t>6:59 PM</t>
+  </si>
+  <si>
+    <t>Friday, Jan 13</t>
+  </si>
+  <si>
+    <t>(SP-LIA)</t>
+  </si>
+  <si>
+    <t>2:20 PM</t>
+  </si>
+  <si>
+    <t>0 hours, -10 minutes</t>
   </si>
 </sst>
 </file>
@@ -383,7 +395,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:M19"/>
+  <dimension ref="A1:M20"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -1090,6 +1102,43 @@
       </c>
       <c r="M19" s="0"/>
     </row>
+    <row r="20">
+      <c r="A20" t="n" s="0">
+        <v>19.0</v>
+      </c>
+      <c r="B20" t="s" s="0">
+        <v>109</v>
+      </c>
+      <c r="C20" t="s" s="0">
+        <v>51</v>
+      </c>
+      <c r="D20" t="s" s="0">
+        <v>52</v>
+      </c>
+      <c r="E20" t="s" s="0">
+        <v>44</v>
+      </c>
+      <c r="F20" t="s" s="0">
+        <v>45</v>
+      </c>
+      <c r="G20" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="H20" t="s" s="0">
+        <v>54</v>
+      </c>
+      <c r="I20" t="s" s="0">
+        <v>110</v>
+      </c>
+      <c r="J20" t="s" s="0">
+        <v>111</v>
+      </c>
+      <c r="K20" s="0"/>
+      <c r="L20" t="s" s="0">
+        <v>112</v>
+      </c>
+      <c r="M20" s="0"/>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
gui added new panel, checkboxes panel and future goals
</commit_message>
<xml_diff>
--- a/DataBase/BZG_Arrivals.xlsx
+++ b/DataBase/BZG_Arrivals.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="125">
   <si>
     <t>NUMBER</t>
   </si>
@@ -351,6 +351,42 @@
   </si>
   <si>
     <t>0 hours, -10 minutes</t>
+  </si>
+  <si>
+    <t>3:30 PM</t>
+  </si>
+  <si>
+    <t>3:16 PM</t>
+  </si>
+  <si>
+    <t>6:55 PM</t>
+  </si>
+  <si>
+    <t>(G-WUKG)</t>
+  </si>
+  <si>
+    <t>6:46 PM</t>
+  </si>
+  <si>
+    <t>0 hours, -9 minutes</t>
+  </si>
+  <si>
+    <t>7:35 PM</t>
+  </si>
+  <si>
+    <t>(EI-EMF)</t>
+  </si>
+  <si>
+    <t>7:11 PM</t>
+  </si>
+  <si>
+    <t>9:25 PM</t>
+  </si>
+  <si>
+    <t>(EI-DWH)</t>
+  </si>
+  <si>
+    <t>9:03 PM</t>
   </si>
 </sst>
 </file>
@@ -395,7 +431,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:M20"/>
+  <dimension ref="A1:M24"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -1139,6 +1175,154 @@
       </c>
       <c r="M20" s="0"/>
     </row>
+    <row r="21">
+      <c r="A21" t="n" s="0">
+        <v>20.0</v>
+      </c>
+      <c r="B21" t="s" s="0">
+        <v>109</v>
+      </c>
+      <c r="C21" t="s" s="0">
+        <v>113</v>
+      </c>
+      <c r="D21" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="E21" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="F21" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="G21" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="H21" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="I21" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="J21" t="s" s="0">
+        <v>114</v>
+      </c>
+      <c r="K21" s="0"/>
+      <c r="L21" t="s" s="0">
+        <v>82</v>
+      </c>
+      <c r="M21" s="0"/>
+    </row>
+    <row r="22">
+      <c r="A22" t="n" s="0">
+        <v>21.0</v>
+      </c>
+      <c r="B22" t="s" s="0">
+        <v>109</v>
+      </c>
+      <c r="C22" t="s" s="0">
+        <v>115</v>
+      </c>
+      <c r="D22" t="s" s="0">
+        <v>35</v>
+      </c>
+      <c r="E22" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="F22" t="s" s="0">
+        <v>36</v>
+      </c>
+      <c r="G22" t="s" s="0">
+        <v>37</v>
+      </c>
+      <c r="H22" t="s" s="0">
+        <v>84</v>
+      </c>
+      <c r="I22" t="s" s="0">
+        <v>116</v>
+      </c>
+      <c r="J22" t="s" s="0">
+        <v>117</v>
+      </c>
+      <c r="K22" s="0"/>
+      <c r="L22" t="s" s="0">
+        <v>118</v>
+      </c>
+      <c r="M22" s="0"/>
+    </row>
+    <row r="23">
+      <c r="A23" t="n" s="0">
+        <v>22.0</v>
+      </c>
+      <c r="B23" t="s" s="0">
+        <v>109</v>
+      </c>
+      <c r="C23" t="s" s="0">
+        <v>119</v>
+      </c>
+      <c r="D23" t="s" s="0">
+        <v>92</v>
+      </c>
+      <c r="E23" t="s" s="0">
+        <v>93</v>
+      </c>
+      <c r="F23" t="s" s="0">
+        <v>94</v>
+      </c>
+      <c r="G23" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="H23" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="I23" t="s" s="0">
+        <v>120</v>
+      </c>
+      <c r="J23" t="s" s="0">
+        <v>121</v>
+      </c>
+      <c r="K23" s="0"/>
+      <c r="L23" t="s" s="0">
+        <v>79</v>
+      </c>
+      <c r="M23" s="0"/>
+    </row>
+    <row r="24">
+      <c r="A24" t="n" s="0">
+        <v>23.0</v>
+      </c>
+      <c r="B24" t="s" s="0">
+        <v>109</v>
+      </c>
+      <c r="C24" t="s" s="0">
+        <v>122</v>
+      </c>
+      <c r="D24" t="s" s="0">
+        <v>65</v>
+      </c>
+      <c r="E24" t="s" s="0">
+        <v>66</v>
+      </c>
+      <c r="F24" t="s" s="0">
+        <v>67</v>
+      </c>
+      <c r="G24" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="H24" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="I24" t="s" s="0">
+        <v>123</v>
+      </c>
+      <c r="J24" t="s" s="0">
+        <v>124</v>
+      </c>
+      <c r="K24" s="0"/>
+      <c r="L24" t="s" s="0">
+        <v>97</v>
+      </c>
+      <c r="M24" s="0"/>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
added downolading from intenet via panel
</commit_message>
<xml_diff>
--- a/DataBase/BZG_Arrivals.xlsx
+++ b/DataBase/BZG_Arrivals.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="132">
   <si>
     <t>NUMBER</t>
   </si>
@@ -387,6 +387,27 @@
   </si>
   <si>
     <t>9:03 PM</t>
+  </si>
+  <si>
+    <t>Saturday, Jan 14</t>
+  </si>
+  <si>
+    <t>(EI-EVH)</t>
+  </si>
+  <si>
+    <t>8:55 AM</t>
+  </si>
+  <si>
+    <t>0 hours, -25 minutes</t>
+  </si>
+  <si>
+    <t>(EI-HMS)</t>
+  </si>
+  <si>
+    <t>9:13 AM</t>
+  </si>
+  <si>
+    <t>0 hours, -17 minutes</t>
   </si>
 </sst>
 </file>
@@ -431,7 +452,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:M24"/>
+  <dimension ref="A1:M26"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -1323,6 +1344,80 @@
       </c>
       <c r="M24" s="0"/>
     </row>
+    <row r="25">
+      <c r="A25" t="n" s="0">
+        <v>24.0</v>
+      </c>
+      <c r="B25" t="s" s="0">
+        <v>125</v>
+      </c>
+      <c r="C25" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="D25" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="E25" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="F25" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="G25" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="H25" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="I25" t="s" s="0">
+        <v>126</v>
+      </c>
+      <c r="J25" t="s" s="0">
+        <v>127</v>
+      </c>
+      <c r="K25" s="0"/>
+      <c r="L25" t="s" s="0">
+        <v>128</v>
+      </c>
+      <c r="M25" s="0"/>
+    </row>
+    <row r="26">
+      <c r="A26" t="n" s="0">
+        <v>25.0</v>
+      </c>
+      <c r="B26" t="s" s="0">
+        <v>125</v>
+      </c>
+      <c r="C26" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="D26" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="E26" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="F26" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="G26" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="H26" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="I26" t="s" s="0">
+        <v>129</v>
+      </c>
+      <c r="J26" t="s" s="0">
+        <v>130</v>
+      </c>
+      <c r="K26" s="0"/>
+      <c r="L26" t="s" s="0">
+        <v>131</v>
+      </c>
+      <c r="M26" s="0"/>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
all graphs added and working
</commit_message>
<xml_diff>
--- a/DataBase/BZG_Arrivals.xlsx
+++ b/DataBase/BZG_Arrivals.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="137">
   <si>
     <t>NUMBER</t>
   </si>
@@ -408,6 +408,21 @@
   </si>
   <si>
     <t>0 hours, -17 minutes</t>
+  </si>
+  <si>
+    <t>Sunday, Jan 15</t>
+  </si>
+  <si>
+    <t>(EI-HGW)</t>
+  </si>
+  <si>
+    <t>0 hours, -15 minutes</t>
+  </si>
+  <si>
+    <t>(SP-LIK)</t>
+  </si>
+  <si>
+    <t>0 hours, -4 minutes</t>
   </si>
 </sst>
 </file>
@@ -452,7 +467,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:M26"/>
+  <dimension ref="A1:M28"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -1418,6 +1433,80 @@
       </c>
       <c r="M26" s="0"/>
     </row>
+    <row r="27">
+      <c r="A27" t="n" s="0">
+        <v>26.0</v>
+      </c>
+      <c r="B27" t="s" s="0">
+        <v>132</v>
+      </c>
+      <c r="C27" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="D27" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="E27" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="F27" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="G27" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="H27" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="I27" t="s" s="0">
+        <v>133</v>
+      </c>
+      <c r="J27" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="K27" s="0"/>
+      <c r="L27" t="s" s="0">
+        <v>134</v>
+      </c>
+      <c r="M27" s="0"/>
+    </row>
+    <row r="28">
+      <c r="A28" t="n" s="0">
+        <v>27.0</v>
+      </c>
+      <c r="B28" t="s" s="0">
+        <v>132</v>
+      </c>
+      <c r="C28" t="s" s="0">
+        <v>51</v>
+      </c>
+      <c r="D28" t="s" s="0">
+        <v>52</v>
+      </c>
+      <c r="E28" t="s" s="0">
+        <v>44</v>
+      </c>
+      <c r="F28" t="s" s="0">
+        <v>45</v>
+      </c>
+      <c r="G28" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="H28" t="s" s="0">
+        <v>54</v>
+      </c>
+      <c r="I28" t="s" s="0">
+        <v>135</v>
+      </c>
+      <c r="J28" t="s" s="0">
+        <v>81</v>
+      </c>
+      <c r="K28" s="0"/>
+      <c r="L28" t="s" s="0">
+        <v>136</v>
+      </c>
+      <c r="M28" s="0"/>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>